<commit_message>
record results from tests in the excel file, and code cleanup. currently the buy and reset tests are working as expected
</commit_message>
<xml_diff>
--- a/Task 1 2 3 Documentation.xlsx
+++ b/Task 1 2 3 Documentation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthewsm\Downloads\Ensek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthewsm\Downloads\Ensek\ExampleAutomationTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7905B2-66FE-4300-90BD-67C65EC0AFC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7451FE0-B14C-4CA4-AC22-B43573AE9E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F43D76C1-831C-45AA-828D-45204C2A73C2}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="127">
   <si>
     <t>Navigation Bar</t>
   </si>
@@ -384,6 +384,54 @@
   </si>
   <si>
     <t>Tested With Id: 5d367abd-9832-400c-9adc-0047368c0422</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Returns Unauthorized Error.</t>
+  </si>
+  <si>
+    <t>Reset Data Test</t>
+  </si>
+  <si>
+    <t>I'm assuming I need an access token. I've attempted to pass the login access_token into the body through an api call but this fails with the same error.</t>
+  </si>
+  <si>
+    <t>This has been confirmed by called the energy api call and seeing there is over 2000 units left, not 10</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Buy Gas</t>
+  </si>
+  <si>
+    <t>The Purchased Units and Quantity Left values are both swapped. Purchase should show 10, and quantity remaining be 2760</t>
+  </si>
+  <si>
+    <t>Buy Nuclear</t>
+  </si>
+  <si>
+    <t>Buy Electricity</t>
+  </si>
+  <si>
+    <t>The Cost has too many decimal places when calculated from the energy cost from the energy api call (Pennies is smallest size). This would be misleading to customers</t>
+  </si>
+  <si>
+    <t>Passed (Automation fail)</t>
+  </si>
+  <si>
+    <t>Not a bug. No nuclear fuel available but the automation test is designed with the intention data will be present. May need a special scenario to check when no fuel available?</t>
   </si>
 </sst>
 </file>
@@ -1122,6 +1170,99 @@
         <a:xfrm>
           <a:off x="1166813" y="12496800"/>
           <a:ext cx="8429687" cy="1362085"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3352799</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>214667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>183839</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B29B69E-3E42-9218-1372-8C4E095B9B3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6553199" y="690917"/>
+          <a:ext cx="10163175" cy="5684172"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>582828</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>29591</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3989FDF4-C489-236D-3C12-6E2F0686402D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="7991475"/>
+          <a:ext cx="12917703" cy="7278116"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2225,38 +2366,107 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20AC1736-1537-4F7D-B6A5-11C285153FD5}">
-  <dimension ref="C4:D5"/>
+  <dimension ref="C1:F72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="71.5703125" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="10"/>
+    <col min="3" max="3" width="18.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="140.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="1" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C2" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C66" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C67" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C71" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D71" s="10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
+    <row r="72" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C72" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D72" s="10" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Internal - Intellectual Property</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated documentation for automation test results
</commit_message>
<xml_diff>
--- a/Task 1 2 3 Documentation.xlsx
+++ b/Task 1 2 3 Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthewsm\Downloads\Ensek\ExampleAutomationTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7451FE0-B14C-4CA4-AC22-B43573AE9E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644F211A-F311-4031-829F-4FF09CD2EDD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{F43D76C1-831C-45AA-828D-45204C2A73C2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F43D76C1-831C-45AA-828D-45204C2A73C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="137">
   <si>
     <t>Navigation Bar</t>
   </si>
@@ -377,15 +377,9 @@
     <t>Extremely bad if stock can be manipulated this way. Finacial loss and energy quantities will need fixing.</t>
   </si>
   <si>
-    <t>Reading a specific Order Id returns an internal Error</t>
-  </si>
-  <si>
     <t>Deleting specific Order Id returns internal Error</t>
   </si>
   <si>
-    <t>Tested With Id: 5d367abd-9832-400c-9adc-0047368c0422</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
@@ -425,13 +419,49 @@
     <t>Buy Electricity</t>
   </si>
   <si>
-    <t>The Cost has too many decimal places when calculated from the energy cost from the energy api call (Pennies is smallest size). This would be misleading to customers</t>
-  </si>
-  <si>
     <t>Passed (Automation fail)</t>
   </si>
   <si>
-    <t>Not a bug. No nuclear fuel available but the automation test is designed with the intention data will be present. May need a special scenario to check when no fuel available?</t>
+    <t>VerifyOrdersTest</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Order Ids older than todays date</t>
+  </si>
+  <si>
+    <t>No Verification checks as the value is dynamic but on 01/12/2023 there were 86 orders older (not including) that date.</t>
+  </si>
+  <si>
+    <t>Read Specific Gas Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cost has too many decimal places when calculated from the energy cost from the energy api call (Pennies is smallest size). </t>
+  </si>
+  <si>
+    <t>This would be misleading to customers</t>
+  </si>
+  <si>
+    <t>Not a bug. No nuclear fuel available but the automation test is designed with the intention data will be present.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> May need a special scenario to check when no fuel available?</t>
+  </si>
+  <si>
+    <t>Did not verify the data of each order, was outside the tests scope but would be added in a real scenario</t>
+  </si>
+  <si>
+    <t>Needs something more solid to verify. E.G. Would need a clean environment and a non parallel test to check this criteria.</t>
+  </si>
+  <si>
+    <t>Returns an Internal Server Error</t>
+  </si>
+  <si>
+    <t>Error implying the feature isnt implemented.</t>
+  </si>
+  <si>
+    <t>The Order ids created were found in the list. Nuclear is not verified as unable to create an order for nuclear energy.</t>
   </si>
 </sst>
 </file>
@@ -1049,15 +1079,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>123910</xdr:colOff>
+      <xdr:colOff>533485</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>171490</xdr:rowOff>
+      <xdr:rowOff>181015</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1080,8 +1110,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1166813" y="3990975"/>
-          <a:ext cx="11611060" cy="5476915"/>
+          <a:off x="1495425" y="3686175"/>
+          <a:ext cx="10868110" cy="5743615"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1093,13 +1123,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>209626</xdr:colOff>
+      <xdr:colOff>533476</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>123843</xdr:rowOff>
     </xdr:to>
@@ -1124,8 +1154,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1166813" y="9782175"/>
-          <a:ext cx="10401376" cy="2476518"/>
+          <a:off x="1495425" y="9820275"/>
+          <a:ext cx="9734626" cy="2600343"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1137,13 +1167,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1147825</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>128650</xdr:colOff>
       <xdr:row>73</xdr:row>
       <xdr:rowOff>95260</xdr:rowOff>
     </xdr:to>
@@ -1168,8 +1198,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1166813" y="12496800"/>
-          <a:ext cx="8429687" cy="1362085"/>
+          <a:off x="1457325" y="12677775"/>
+          <a:ext cx="7948675" cy="1428760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1185,16 +1215,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>3352799</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>214667</xdr:rowOff>
+      <xdr:rowOff>128942</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>183839</xdr:rowOff>
+      <xdr:rowOff>98114</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1217,7 +1247,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6553199" y="690917"/>
+          <a:off x="7677149" y="605192"/>
           <a:ext cx="10163175" cy="5684172"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1229,14 +1259,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>582828</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>373278</xdr:colOff>
       <xdr:row>64</xdr:row>
       <xdr:rowOff>29591</xdr:rowOff>
     </xdr:to>
@@ -1573,8 +1603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1777EEED-114F-4CA1-AEF5-8D5EFB62AD4F}">
   <dimension ref="A2:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1990,13 +2020,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBBA4F4B-20EA-4C3B-B6B7-C069FA98FAE6}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="82.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
@@ -2186,7 +2216,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,7 +2224,7 @@
     <col min="1" max="1" width="68.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="93.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="176" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2366,99 +2396,145 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20AC1736-1537-4F7D-B6A5-11C285153FD5}">
-  <dimension ref="C1:F72"/>
+  <dimension ref="B1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="10"/>
-    <col min="3" max="3" width="18.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="140.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="9.140625" style="10"/>
+    <col min="2" max="2" width="65.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="143.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
+        <v>109</v>
+      </c>
       <c r="C1" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="E1" s="10" t="s">
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C2" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>119</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="F2" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="10" t="s">
+        <v>118</v>
+      </c>
       <c r="C32" s="10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>119</v>
       </c>
       <c r="E32" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="C66" s="10" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C66" s="10" t="s">
-        <v>123</v>
-      </c>
       <c r="D66" s="10" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B67" s="10" t="s">
+        <v>120</v>
+      </c>
       <c r="C67" s="10" t="s">
         <v>122</v>
       </c>
       <c r="D67" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B70" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B71" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="C71" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D71" s="10" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C71" s="10" t="s">
+      <c r="E71" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B73" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B74" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D71" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C72" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>110</v>
+      <c r="C74" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>